<commit_message>
focus on data sheet
</commit_message>
<xml_diff>
--- a/UserTestEval/Data/Rawdata.xlsx
+++ b/UserTestEval/Data/Rawdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katha\Documents\uni\Evaluation-of-templates-for-requirements-documentation\UserTestEval\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katha\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9647B595-3A8A-4BFF-B22B-BB4DB4BEF349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5287A3E-2021-4A12-90CB-FA0F9C7BD33A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="3975" windowWidth="25440" windowHeight="15270" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AllData" sheetId="2" r:id="rId1"/>
@@ -26,88 +26,53 @@
     <definedName name="_xlchart.v1.10" hidden="1">Ranking!$C$2:$C$216</definedName>
     <definedName name="_xlchart.v1.11" hidden="1">Ranking!$D$1</definedName>
     <definedName name="_xlchart.v1.12" hidden="1">Ranking!$D$2:$D$216</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Ranking!$A$2:$A$216</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Ranking!$A$2:$A$211</definedName>
     <definedName name="_xlchart.v1.14" hidden="1">Ranking!$B$1</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Ranking!$B$2:$B$216</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Ranking!$B$2:$B$211</definedName>
     <definedName name="_xlchart.v1.16" hidden="1">Ranking!$C$1</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Ranking!$C$2:$C$216</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Ranking!$C$2:$C$211</definedName>
     <definedName name="_xlchart.v1.18" hidden="1">Ranking!$D$1</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Ranking!$D$2:$D$216</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">Ranking!$D$2:$D$211</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">Ranking!$C$1</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Ranking!$A$2:$A$216</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Ranking!$B$1</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Ranking!$B$2:$B$216</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Ranking!$C$1</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Ranking!$C$2:$C$216</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Ranking!$D$1</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Ranking!$D$2:$D$216</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">Ranking!$A$2:$A$211</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">Ranking!$A$2:$A$216</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">Ranking!$B$1</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">Time!$A$2:$A$43</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Time!$B$1</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">Time!$B$2:$B$43</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">Time!$C$1</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">Time!$C$2:$C$43</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">Time!$A$2:$A$44</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">Time!$B$1</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">Time!$B$2:$B$44</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">Time!$C$1</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">Time!$C$2:$C$44</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">Ranking!$C$2:$C$216</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">Ranking!$B$2:$B$211</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">Ranking!$B$2:$B$216</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">Ranking!$C$1</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">Ranking!$C$2:$C$211</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">Ranking!$C$2:$C$216</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">Ranking!$D$1</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">Ranking!$D$2:$D$211</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">Ranking!$D$2:$D$216</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">Ranking!$A$2:$A$216</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">Ranking!$B$1</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">Time!$D$3:$D$43</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">Time!$E$3:$E$43</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">Time!$F$2:$F$43</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">Time!$G$1</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">Time!$G$2:$G$43</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">QualityReview!$A$2:$B$13</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">QualityReview!$C$1</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">QualityReview!$C$2:$C$13</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">QualityReview!$D$1</definedName>
+    <definedName name="_xlchart.v1.39" hidden="1">QualityReview!$D$2:$D$13</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">Ranking!$D$1</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">Ranking!$B$2:$B$216</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">Ranking!$C$1</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">Ranking!$C$2:$C$216</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">Ranking!$D$1</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">Ranking!$D$2:$D$216</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">Ranking!$A$2:$A$216</definedName>
-    <definedName name="_xlchart.v1.46" hidden="1">Ranking!$B$1</definedName>
-    <definedName name="_xlchart.v1.47" hidden="1">Ranking!$B$2:$B$216</definedName>
-    <definedName name="_xlchart.v1.48" hidden="1">Ranking!$C$1</definedName>
-    <definedName name="_xlchart.v1.49" hidden="1">Ranking!$C$2:$C$216</definedName>
+    <definedName name="_xlchart.v1.40" hidden="1">QualityReview!$E$1</definedName>
+    <definedName name="_xlchart.v1.41" hidden="1">QualityReview!$E$2:$E$13</definedName>
+    <definedName name="_xlchart.v1.42" hidden="1">QualityReview!$F$1</definedName>
+    <definedName name="_xlchart.v1.43" hidden="1">QualityReview!$F$2:$F$13</definedName>
+    <definedName name="_xlchart.v1.44" hidden="1">QualityReview!$A$23:$A$34</definedName>
+    <definedName name="_xlchart.v1.45" hidden="1">QualityReview!$C$22</definedName>
+    <definedName name="_xlchart.v1.46" hidden="1">QualityReview!$C$23:$C$34</definedName>
+    <definedName name="_xlchart.v1.47" hidden="1">QualityReview!$D$22</definedName>
+    <definedName name="_xlchart.v1.48" hidden="1">QualityReview!$D$23:$D$34</definedName>
+    <definedName name="_xlchart.v1.49" hidden="1">QualityReview!$E$22</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">Ranking!$D$2:$D$216</definedName>
-    <definedName name="_xlchart.v1.50" hidden="1">Ranking!$D$1</definedName>
-    <definedName name="_xlchart.v1.51" hidden="1">Ranking!$D$2:$D$216</definedName>
-    <definedName name="_xlchart.v1.52" hidden="1">Time!$D$3:$D$43</definedName>
-    <definedName name="_xlchart.v1.53" hidden="1">Time!$E$3:$E$43</definedName>
-    <definedName name="_xlchart.v1.54" hidden="1">Time!$F$2:$F$43</definedName>
-    <definedName name="_xlchart.v1.55" hidden="1">Time!$G$1</definedName>
-    <definedName name="_xlchart.v1.56" hidden="1">Time!$G$2:$G$43</definedName>
-    <definedName name="_xlchart.v1.57" hidden="1">Time!$A$2:$A$43</definedName>
-    <definedName name="_xlchart.v1.58" hidden="1">Time!$B$1</definedName>
-    <definedName name="_xlchart.v1.59" hidden="1">Time!$B$2:$B$43</definedName>
+    <definedName name="_xlchart.v1.50" hidden="1">QualityReview!$E$23:$E$34</definedName>
+    <definedName name="_xlchart.v1.51" hidden="1">QualityReview!$F$22</definedName>
+    <definedName name="_xlchart.v1.52" hidden="1">QualityReview!$F$23:$F$34</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">Ranking!$A$2:$A$216</definedName>
-    <definedName name="_xlchart.v1.60" hidden="1">Time!$C$1</definedName>
-    <definedName name="_xlchart.v1.61" hidden="1">Time!$C$2:$C$43</definedName>
-    <definedName name="_xlchart.v1.62" hidden="1">Time!$A$2:$A$44</definedName>
-    <definedName name="_xlchart.v1.63" hidden="1">Time!$B$1</definedName>
-    <definedName name="_xlchart.v1.64" hidden="1">Time!$B$2:$B$44</definedName>
-    <definedName name="_xlchart.v1.65" hidden="1">Time!$C$1</definedName>
-    <definedName name="_xlchart.v1.66" hidden="1">Time!$C$2:$C$44</definedName>
-    <definedName name="_xlchart.v1.67" hidden="1">Time!$F$2:$F$43</definedName>
-    <definedName name="_xlchart.v1.68" hidden="1">Time!$G$1</definedName>
-    <definedName name="_xlchart.v1.69" hidden="1">Time!$G$2:$G$43</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">Ranking!$B$1</definedName>
-    <definedName name="_xlchart.v1.70" hidden="1">QualityReview!$A$2:$B$13</definedName>
-    <definedName name="_xlchart.v1.71" hidden="1">QualityReview!$C$1</definedName>
-    <definedName name="_xlchart.v1.72" hidden="1">QualityReview!$C$2:$C$13</definedName>
-    <definedName name="_xlchart.v1.73" hidden="1">QualityReview!$D$1</definedName>
-    <definedName name="_xlchart.v1.74" hidden="1">QualityReview!$D$2:$D$13</definedName>
-    <definedName name="_xlchart.v1.75" hidden="1">QualityReview!$E$1</definedName>
-    <definedName name="_xlchart.v1.76" hidden="1">QualityReview!$E$2:$E$13</definedName>
-    <definedName name="_xlchart.v1.77" hidden="1">QualityReview!$F$1</definedName>
-    <definedName name="_xlchart.v1.78" hidden="1">QualityReview!$F$2:$F$13</definedName>
-    <definedName name="_xlchart.v1.79" hidden="1">QualityReview!$A$23:$A$34</definedName>
     <definedName name="_xlchart.v1.8" hidden="1">Ranking!$B$2:$B$216</definedName>
-    <definedName name="_xlchart.v1.80" hidden="1">QualityReview!$C$22</definedName>
-    <definedName name="_xlchart.v1.81" hidden="1">QualityReview!$C$23:$C$34</definedName>
-    <definedName name="_xlchart.v1.82" hidden="1">QualityReview!$D$22</definedName>
-    <definedName name="_xlchart.v1.83" hidden="1">QualityReview!$D$23:$D$34</definedName>
-    <definedName name="_xlchart.v1.84" hidden="1">QualityReview!$E$22</definedName>
-    <definedName name="_xlchart.v1.85" hidden="1">QualityReview!$E$23:$E$34</definedName>
-    <definedName name="_xlchart.v1.86" hidden="1">QualityReview!$F$22</definedName>
-    <definedName name="_xlchart.v1.87" hidden="1">QualityReview!$F$23:$F$34</definedName>
     <definedName name="_xlchart.v1.9" hidden="1">Ranking!$C$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -2849,26 +2814,26 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.38</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.40</cx:f>
+        <cx:f>_xlchart.v1.8</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.38</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.42</cx:f>
+        <cx:f>_xlchart.v1.10</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.38</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.44</cx:f>
+        <cx:f>_xlchart.v1.12</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2885,7 +2850,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{9F5367F5-9D47-46AD-B596-0EFA7A478491}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.39</cx:f>
+              <cx:f>_xlchart.v1.7</cx:f>
               <cx:v>free</cx:v>
             </cx:txData>
           </cx:tx>
@@ -2898,7 +2863,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{5A5F7C4B-719B-40B2-B332-D53E44E122AB}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.41</cx:f>
+              <cx:f>_xlchart.v1.9</cx:f>
               <cx:v>EARS</cx:v>
             </cx:txData>
           </cx:tx>
@@ -2911,7 +2876,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{55F26920-8301-4343-A252-521020BA38E7}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.43</cx:f>
+              <cx:f>_xlchart.v1.11</cx:f>
               <cx:v>MASTER</cx:v>
             </cx:txData>
           </cx:tx>
@@ -3129,26 +3094,26 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.27</cx:f>
+        <cx:f>_xlchart.v1.13</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.30</cx:f>
+        <cx:f>_xlchart.v1.15</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.27</cx:f>
+        <cx:f>_xlchart.v1.13</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.33</cx:f>
+        <cx:f>_xlchart.v1.17</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.27</cx:f>
+        <cx:f>_xlchart.v1.13</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.36</cx:f>
+        <cx:f>_xlchart.v1.19</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -3165,7 +3130,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{CB637DB2-7F16-46BD-BECF-B186D777151E}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.29</cx:f>
+              <cx:f>_xlchart.v1.14</cx:f>
               <cx:v>free</cx:v>
             </cx:txData>
           </cx:tx>
@@ -3178,7 +3143,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{C908A5A9-6C1E-4C60-B384-5224CE0FDF11}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.32</cx:f>
+              <cx:f>_xlchart.v1.16</cx:f>
               <cx:v>EARS</cx:v>
             </cx:txData>
           </cx:tx>
@@ -3191,7 +3156,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{B19EAA18-68A6-4A27-8698-E85CD5441D2F}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.35</cx:f>
+              <cx:f>_xlchart.v1.18</cx:f>
               <cx:v>MASTER</cx:v>
             </cx:txData>
           </cx:tx>
@@ -3409,18 +3374,18 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.62</cx:f>
+        <cx:f>_xlchart.v1.25</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.64</cx:f>
+        <cx:f>_xlchart.v1.27</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.62</cx:f>
+        <cx:f>_xlchart.v1.25</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.66</cx:f>
+        <cx:f>_xlchart.v1.29</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -3430,7 +3395,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{A7955AD6-7364-416F-A82A-58A1F76E455D}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.63</cx:f>
+              <cx:f>_xlchart.v1.26</cx:f>
               <cx:v>EARS</cx:v>
             </cx:txData>
           </cx:tx>
@@ -3455,7 +3420,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{6C77626C-2690-4B4A-A861-13008AE16954}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.65</cx:f>
+              <cx:f>_xlchart.v1.28</cx:f>
               <cx:v>MASTER</cx:v>
             </cx:txData>
           </cx:tx>
@@ -3503,18 +3468,18 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.57</cx:f>
+        <cx:f>_xlchart.v1.20</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.59</cx:f>
+        <cx:f>_xlchart.v1.22</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.57</cx:f>
+        <cx:f>_xlchart.v1.20</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.61</cx:f>
+        <cx:f>_xlchart.v1.24</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -3524,7 +3489,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{F8EE3ECA-F2A0-4D89-B44B-860DB1DF4BFB}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.58</cx:f>
+              <cx:f>_xlchart.v1.21</cx:f>
               <cx:v>EARS</cx:v>
             </cx:txData>
           </cx:tx>
@@ -3549,7 +3514,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{5FE71DA6-CBA9-45DB-9983-296628AFA7E5}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.60</cx:f>
+              <cx:f>_xlchart.v1.23</cx:f>
               <cx:v>MASTER</cx:v>
             </cx:txData>
           </cx:tx>
@@ -3597,10 +3562,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.54</cx:f>
+        <cx:f>_xlchart.v1.32</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.56</cx:f>
+        <cx:f>_xlchart.v1.34</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -3617,7 +3582,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{4F766D4F-6C7B-48A5-BD5A-CAC0903FDF09}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.55</cx:f>
+              <cx:f>_xlchart.v1.33</cx:f>
               <cx:v>Total</cx:v>
             </cx:txData>
           </cx:tx>
@@ -3653,10 +3618,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.52</cx:f>
+        <cx:f>_xlchart.v1.30</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.53</cx:f>
+        <cx:f>_xlchart.v1.31</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -3696,34 +3661,34 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.70</cx:f>
+        <cx:f>_xlchart.v1.35</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.72</cx:f>
+        <cx:f>_xlchart.v1.37</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.70</cx:f>
+        <cx:f>_xlchart.v1.35</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.74</cx:f>
+        <cx:f>_xlchart.v1.39</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.70</cx:f>
+        <cx:f>_xlchart.v1.35</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.76</cx:f>
+        <cx:f>_xlchart.v1.41</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.70</cx:f>
+        <cx:f>_xlchart.v1.35</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.78</cx:f>
+        <cx:f>_xlchart.v1.43</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -3733,7 +3698,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{77F25C24-85DD-4A54-A7D1-D94F6F8E168F}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.71</cx:f>
+              <cx:f>_xlchart.v1.36</cx:f>
               <cx:v>vague</cx:v>
             </cx:txData>
           </cx:tx>
@@ -3746,7 +3711,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{14EEBEFD-7F9A-4E97-87C1-E8349BC99461}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.73</cx:f>
+              <cx:f>_xlchart.v1.38</cx:f>
               <cx:v>incomplete</cx:v>
             </cx:txData>
           </cx:tx>
@@ -3759,7 +3724,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{E056748F-24A3-4E02-8A68-8AAC77CCAFCB}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.75</cx:f>
+              <cx:f>_xlchart.v1.40</cx:f>
               <cx:v>incorrect</cx:v>
             </cx:txData>
           </cx:tx>
@@ -3772,7 +3737,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{672FCDD8-5A6D-4A50-BC3E-796BD53E6BB0}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.77</cx:f>
+              <cx:f>_xlchart.v1.42</cx:f>
               <cx:v>none</cx:v>
             </cx:txData>
           </cx:tx>
@@ -3859,34 +3824,34 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.79</cx:f>
+        <cx:f>_xlchart.v1.44</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.81</cx:f>
+        <cx:f>_xlchart.v1.46</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.79</cx:f>
+        <cx:f>_xlchart.v1.44</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.83</cx:f>
+        <cx:f>_xlchart.v1.48</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.79</cx:f>
+        <cx:f>_xlchart.v1.44</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.85</cx:f>
+        <cx:f>_xlchart.v1.50</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.79</cx:f>
+        <cx:f>_xlchart.v1.44</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.87</cx:f>
+        <cx:f>_xlchart.v1.52</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -3896,7 +3861,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{027BD639-9B66-4C1E-AA91-895916F501ED}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.80</cx:f>
+              <cx:f>_xlchart.v1.45</cx:f>
               <cx:v>vague</cx:v>
             </cx:txData>
           </cx:tx>
@@ -3909,7 +3874,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{72CB3FFF-E10B-447F-9F63-53AD6057415C}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.82</cx:f>
+              <cx:f>_xlchart.v1.47</cx:f>
               <cx:v>incomplete</cx:v>
             </cx:txData>
           </cx:tx>
@@ -3922,7 +3887,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{53BA64B2-98E1-43B8-8AF0-164E805B40AA}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.84</cx:f>
+              <cx:f>_xlchart.v1.49</cx:f>
               <cx:v>incorrect</cx:v>
             </cx:txData>
           </cx:tx>
@@ -3935,7 +3900,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{AFDE7047-C063-4660-AE6C-95B79B0FA1CB}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.86</cx:f>
+              <cx:f>_xlchart.v1.51</cx:f>
               <cx:v>none</cx:v>
             </cx:txData>
           </cx:tx>
@@ -11359,7 +11324,7 @@
           <xdr:spPr>
             <a:xfrm>
               <a:off x="3752850" y="161925"/>
-              <a:ext cx="4572000" cy="2600325"/>
+              <a:ext cx="4572000" cy="2595563"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -11436,7 +11401,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3838574" y="3009900"/>
+              <a:off x="3838574" y="3005138"/>
               <a:ext cx="4572000" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -11514,7 +11479,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="8505825" y="3057525"/>
+              <a:off x="8505825" y="3052763"/>
               <a:ext cx="4572000" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -11597,7 +11562,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5000625" y="457200"/>
+              <a:off x="6677025" y="452438"/>
               <a:ext cx="4572000" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -11675,7 +11640,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5038725" y="3695700"/>
+              <a:off x="6715125" y="3690938"/>
               <a:ext cx="4572000" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -11753,7 +11718,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="5895975" y="6905625"/>
+              <a:off x="6734175" y="6900863"/>
               <a:ext cx="4572000" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -11831,7 +11796,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="1828800" y="7724775"/>
+              <a:off x="1828800" y="7720013"/>
               <a:ext cx="4572000" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -12030,8 +11995,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6715124" y="6515100"/>
-              <a:ext cx="4562476" cy="2590800"/>
+              <a:off x="6710362" y="6515100"/>
+              <a:ext cx="4567238" cy="2590800"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -13085,9 +13050,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BS44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A54" sqref="A54:XFD54"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -13316,7 +13279,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:71" ht="319.14999999999998" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:71" ht="306.39999999999998" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>174</v>
       </c>
@@ -13528,7 +13491,7 @@
         <v>0.45277777777777778</v>
       </c>
     </row>
-    <row r="3" spans="1:71" ht="293.64999999999998" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:71" ht="280.89999999999998" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>171</v>
       </c>
@@ -14180,7 +14143,7 @@
         <v>0.44722222222222219</v>
       </c>
     </row>
-    <row r="6" spans="1:71" ht="357.4" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:71" ht="344.65" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>174</v>
       </c>
@@ -14384,7 +14347,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="7" spans="1:71" ht="382.9" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:71" ht="370.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>174</v>
       </c>
@@ -14594,7 +14557,7 @@
         <v>0.45208333333333334</v>
       </c>
     </row>
-    <row r="8" spans="1:71" ht="409.6" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:71" ht="408.4" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>174</v>
       </c>
@@ -15658,7 +15621,7 @@
         <v>0.45555555555555555</v>
       </c>
     </row>
-    <row r="13" spans="1:71" ht="370.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:71" ht="357.4" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>174</v>
       </c>
@@ -16500,7 +16463,7 @@
         <v>0.55902777777777779</v>
       </c>
     </row>
-    <row r="17" spans="1:71" ht="395.65" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:71" ht="382.9" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>171</v>
       </c>
@@ -17352,7 +17315,7 @@
         <v>0.4548611111111111</v>
       </c>
     </row>
-    <row r="21" spans="1:71" ht="370.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:71" ht="357.4" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>174</v>
       </c>
@@ -17776,7 +17739,7 @@
         <v>0.45277777777777778</v>
       </c>
     </row>
-    <row r="23" spans="1:71" ht="344.65" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:71" ht="331.9" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
         <v>174</v>
       </c>
@@ -19036,7 +18999,7 @@
         <v>0.45277777777777778</v>
       </c>
     </row>
-    <row r="29" spans="1:71" ht="370.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:71" ht="357.4" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
         <v>174</v>
       </c>
@@ -21154,7 +21117,7 @@
         <v>0.55138888888888882</v>
       </c>
     </row>
-    <row r="39" spans="1:71" ht="217.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:71" ht="204.4" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="1" t="s">
         <v>174</v>
       </c>
@@ -21358,7 +21321,7 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="40" spans="1:71" ht="344.65" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:71" ht="331.9" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="1" t="s">
         <v>174</v>
       </c>
@@ -21576,7 +21539,7 @@
         <v>0.47222222222222227</v>
       </c>
     </row>
-    <row r="41" spans="1:71" ht="370.15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:71" ht="357.4" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="1" t="s">
         <v>174</v>
       </c>
@@ -22216,7 +22179,7 @@
         <v>0.45694444444444443</v>
       </c>
     </row>
-    <row r="44" spans="1:71" ht="191.65" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:71" ht="178.9" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="1" t="s">
         <v>174</v>
       </c>
@@ -27457,7 +27420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FC39F50-491B-4545-9F82-98E8A6306DE7}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
@@ -27500,7 +27463,7 @@
         <v>6.9444444444444753E-3</v>
       </c>
       <c r="D2" s="8" t="str">
-        <f>A2</f>
+        <f t="shared" ref="D2:D44" si="0">A2</f>
         <v>Student</v>
       </c>
       <c r="E2" s="8">
@@ -27508,7 +27471,7 @@
         <v>-0.18541666666666662</v>
       </c>
       <c r="F2" s="8" t="str">
-        <f>A2</f>
+        <f t="shared" ref="F2:F44" si="1">A2</f>
         <v>Student</v>
       </c>
       <c r="G2" s="8">
@@ -27530,7 +27493,7 @@
         <v>2.7777777777777679E-3</v>
       </c>
       <c r="D3" s="8" t="str">
-        <f>A3</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E3" s="8">
@@ -27538,7 +27501,7 @@
         <v>2.0833333333333259E-3</v>
       </c>
       <c r="F3" s="8" t="str">
-        <f>A3</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G3" s="8">
@@ -27560,7 +27523,7 @@
         <v>2.0833333333333814E-3</v>
       </c>
       <c r="D4" s="8" t="str">
-        <f>A4</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E4" s="8">
@@ -27568,7 +27531,7 @@
         <v>5.5555555555555358E-3</v>
       </c>
       <c r="F4" s="8" t="str">
-        <f>A4</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G4" s="8">
@@ -27590,7 +27553,7 @@
         <v>3.4722222222222099E-3</v>
       </c>
       <c r="D5" s="8" t="str">
-        <f>A5</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E5" s="8">
@@ -27598,7 +27561,7 @@
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="F5" s="8" t="str">
-        <f>A5</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G5" s="8">
@@ -27620,7 +27583,7 @@
         <v>8.3333333333334147E-3</v>
       </c>
       <c r="D6" s="8" t="str">
-        <f>A6</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E6" s="8">
@@ -27628,7 +27591,7 @@
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="F6" s="8" t="str">
-        <f>A6</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G6" s="8">
@@ -27650,7 +27613,7 @@
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="D7" s="8" t="str">
-        <f>A7</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E7" s="8">
@@ -27658,7 +27621,7 @@
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="F7" s="8" t="str">
-        <f>A7</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G7" s="8">
@@ -27680,7 +27643,7 @@
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="D8" s="8" t="str">
-        <f>A8</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E8" s="8">
@@ -27688,7 +27651,7 @@
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="F8" s="8" t="str">
-        <f>A8</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G8" s="8">
@@ -27710,7 +27673,7 @@
         <v>2.0833333333333814E-3</v>
       </c>
       <c r="D9" s="8" t="str">
-        <f>A9</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E9" s="8">
@@ -27718,7 +27681,7 @@
         <v>6.9444444444445308E-3</v>
       </c>
       <c r="F9" s="8" t="str">
-        <f>A9</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G9" s="8">
@@ -27740,7 +27703,7 @@
         <v>2.0833333333333259E-3</v>
       </c>
       <c r="D10" s="8" t="str">
-        <f>A10</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E10" s="8">
@@ -27748,7 +27711,7 @@
         <v>8.3333333333333037E-3</v>
       </c>
       <c r="F10" s="8" t="str">
-        <f>A10</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G10" s="8">
@@ -27770,7 +27733,7 @@
         <v>4.8611111111110938E-3</v>
       </c>
       <c r="D11" s="8" t="str">
-        <f>A11</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E11" s="8">
@@ -27778,7 +27741,7 @@
         <v>8.3333333333333037E-3</v>
       </c>
       <c r="F11" s="8" t="str">
-        <f>A11</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G11" s="8">
@@ -27800,7 +27763,7 @@
         <v>3.4722222222222099E-3</v>
       </c>
       <c r="D12" s="8" t="str">
-        <f>A12</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E12" s="8">
@@ -27808,7 +27771,7 @@
         <v>9.0277777777777457E-3</v>
       </c>
       <c r="F12" s="8" t="str">
-        <f>A12</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G12" s="8">
@@ -27830,7 +27793,7 @@
         <v>2.7777777777777679E-3</v>
       </c>
       <c r="D13" s="8" t="str">
-        <f>A13</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E13" s="8">
@@ -27838,7 +27801,7 @@
         <v>9.0277777777778012E-3</v>
       </c>
       <c r="F13" s="8" t="str">
-        <f>A13</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G13" s="8">
@@ -27860,7 +27823,7 @@
         <v>3.4722222222222099E-3</v>
       </c>
       <c r="D14" s="8" t="str">
-        <f>A14</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E14" s="8">
@@ -27868,7 +27831,7 @@
         <v>9.0277777777778012E-3</v>
       </c>
       <c r="F14" s="8" t="str">
-        <f>A14</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G14" s="8">
@@ -27890,7 +27853,7 @@
         <v>5.5555555555555358E-3</v>
       </c>
       <c r="D15" s="8" t="str">
-        <f>A15</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E15" s="8">
@@ -27898,7 +27861,7 @@
         <v>9.0277777777778012E-3</v>
       </c>
       <c r="F15" s="8" t="str">
-        <f>A15</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G15" s="8">
@@ -27920,7 +27883,7 @@
         <v>4.1666666666666519E-3</v>
       </c>
       <c r="D16" s="8" t="str">
-        <f>A16</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E16" s="8">
@@ -27928,7 +27891,7 @@
         <v>9.7222222222221877E-3</v>
       </c>
       <c r="F16" s="8" t="str">
-        <f>A16</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G16" s="8">
@@ -27950,7 +27913,7 @@
         <v>2.7777777777777679E-3</v>
       </c>
       <c r="D17" s="8" t="str">
-        <f>A17</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E17" s="8">
@@ -27958,7 +27921,7 @@
         <v>1.0416666666666685E-2</v>
       </c>
       <c r="F17" s="8" t="str">
-        <f>A17</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G17" s="8">
@@ -27980,7 +27943,7 @@
         <v>4.8611111111112049E-3</v>
       </c>
       <c r="D18" s="8" t="str">
-        <f>A18</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E18" s="8">
@@ -27988,7 +27951,7 @@
         <v>1.1111111111111072E-2</v>
       </c>
       <c r="F18" s="8" t="str">
-        <f>A18</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G18" s="8">
@@ -28010,7 +27973,7 @@
         <v>8.3333333333334147E-3</v>
       </c>
       <c r="D19" s="8" t="str">
-        <f>A19</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E19" s="8">
@@ -28018,7 +27981,7 @@
         <v>1.1805555555555514E-2</v>
       </c>
       <c r="F19" s="8" t="str">
-        <f>A19</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G19" s="8">
@@ -28040,7 +28003,7 @@
         <v>2.0833333333333259E-3</v>
       </c>
       <c r="D20" s="8" t="str">
-        <f>A20</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E20" s="8">
@@ -28048,7 +28011,7 @@
         <v>1.1805555555555569E-2</v>
       </c>
       <c r="F20" s="8" t="str">
-        <f>A20</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G20" s="8">
@@ -28070,7 +28033,7 @@
         <v>2.0833333333333259E-3</v>
       </c>
       <c r="D21" s="8" t="str">
-        <f>A21</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E21" s="8">
@@ -28078,7 +28041,7 @@
         <v>1.2500000000000067E-2</v>
       </c>
       <c r="F21" s="8" t="str">
-        <f>A21</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G21" s="8">
@@ -28100,7 +28063,7 @@
         <v>4.8611111111111494E-3</v>
       </c>
       <c r="D22" s="8" t="str">
-        <f>A22</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E22" s="8">
@@ -28108,7 +28071,7 @@
         <v>1.2500000000000067E-2</v>
       </c>
       <c r="F22" s="8" t="str">
-        <f>A22</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G22" s="8">
@@ -28130,7 +28093,7 @@
         <v>5.5555555555556468E-3</v>
       </c>
       <c r="D23" s="8" t="str">
-        <f>A23</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E23" s="8">
@@ -28138,7 +28101,7 @@
         <v>1.388888888888884E-2</v>
       </c>
       <c r="F23" s="8" t="str">
-        <f>A23</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G23" s="8">
@@ -28160,7 +28123,7 @@
         <v>5.5555555555555358E-3</v>
       </c>
       <c r="D24" s="8" t="str">
-        <f>A24</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E24" s="8">
@@ -28168,7 +28131,7 @@
         <v>1.3888888888888951E-2</v>
       </c>
       <c r="F24" s="8" t="str">
-        <f>A24</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G24" s="8">
@@ -28190,7 +28153,7 @@
         <v>5.5555555555555358E-3</v>
       </c>
       <c r="D25" s="8" t="str">
-        <f>A25</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E25" s="8">
@@ -28198,7 +28161,7 @@
         <v>1.3888888888888951E-2</v>
       </c>
       <c r="F25" s="8" t="str">
-        <f>A25</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G25" s="8">
@@ -28220,7 +28183,7 @@
         <v>4.8611111111110383E-3</v>
       </c>
       <c r="D26" s="8" t="str">
-        <f>A26</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E26" s="8">
@@ -28228,7 +28191,7 @@
         <v>1.4583333333333337E-2</v>
       </c>
       <c r="F26" s="8" t="str">
-        <f>A26</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G26" s="8">
@@ -28250,7 +28213,7 @@
         <v>6.2500000000000333E-3</v>
       </c>
       <c r="D27" s="8" t="str">
-        <f>A27</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E27" s="8">
@@ -28258,7 +28221,7 @@
         <v>1.4583333333333337E-2</v>
       </c>
       <c r="F27" s="8" t="str">
-        <f>A27</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G27" s="8">
@@ -28280,7 +28243,7 @@
         <v>2.7777777777778234E-3</v>
       </c>
       <c r="D28" s="8" t="str">
-        <f>A28</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E28" s="8">
@@ -28288,7 +28251,7 @@
         <v>1.4583333333333337E-2</v>
       </c>
       <c r="F28" s="8" t="str">
-        <f>A28</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G28" s="8">
@@ -28310,7 +28273,7 @@
         <v>6.9444444444444753E-3</v>
       </c>
       <c r="D29" s="8" t="str">
-        <f>A29</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E29" s="8">
@@ -28318,7 +28281,7 @@
         <v>1.5277777777777779E-2</v>
       </c>
       <c r="F29" s="8" t="str">
-        <f>A29</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G29" s="8">
@@ -28340,7 +28303,7 @@
         <v>4.8611111111111494E-3</v>
       </c>
       <c r="D30" s="8" t="str">
-        <f>A30</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E30" s="8">
@@ -28348,7 +28311,7 @@
         <v>1.5277777777777779E-2</v>
       </c>
       <c r="F30" s="8" t="str">
-        <f>A30</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G30" s="8">
@@ -28370,7 +28333,7 @@
         <v>4.8611111111111494E-3</v>
       </c>
       <c r="D31" s="8" t="str">
-        <f>A31</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E31" s="8">
@@ -28378,7 +28341,7 @@
         <v>1.5277777777777779E-2</v>
       </c>
       <c r="F31" s="8" t="str">
-        <f>A31</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G31" s="8">
@@ -28400,7 +28363,7 @@
         <v>3.4722222222222099E-3</v>
       </c>
       <c r="D32" s="8" t="str">
-        <f>A32</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E32" s="8">
@@ -28408,7 +28371,7 @@
         <v>1.5972222222222221E-2</v>
       </c>
       <c r="F32" s="8" t="str">
-        <f>A32</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G32" s="8">
@@ -28430,7 +28393,7 @@
         <v>6.2499999999999778E-3</v>
       </c>
       <c r="D33" s="8" t="str">
-        <f>A33</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E33" s="8">
@@ -28438,7 +28401,7 @@
         <v>1.5972222222222276E-2</v>
       </c>
       <c r="F33" s="8" t="str">
-        <f>A33</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G33" s="8">
@@ -28460,7 +28423,7 @@
         <v>5.5555555555555358E-3</v>
       </c>
       <c r="D34" s="8" t="str">
-        <f>A34</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E34" s="8">
@@ -28468,7 +28431,7 @@
         <v>1.6666666666666718E-2</v>
       </c>
       <c r="F34" s="8" t="str">
-        <f>A34</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G34" s="8">
@@ -28490,7 +28453,7 @@
         <v>4.8611111111111494E-3</v>
       </c>
       <c r="D35" s="8" t="str">
-        <f>A35</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E35" s="8">
@@ -28498,7 +28461,7 @@
         <v>1.6666666666666718E-2</v>
       </c>
       <c r="F35" s="8" t="str">
-        <f>A35</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G35" s="8">
@@ -28520,7 +28483,7 @@
         <v>5.5555555555555358E-3</v>
       </c>
       <c r="D36" s="8" t="str">
-        <f>A36</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E36" s="8">
@@ -28528,7 +28491,7 @@
         <v>1.8055555555555547E-2</v>
       </c>
       <c r="F36" s="8" t="str">
-        <f>A36</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G36" s="8">
@@ -28550,7 +28513,7 @@
         <v>4.8611111111110938E-3</v>
       </c>
       <c r="D37" s="8" t="str">
-        <f>A37</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E37" s="8">
@@ -28558,7 +28521,7 @@
         <v>1.9444444444444486E-2</v>
       </c>
       <c r="F37" s="8" t="str">
-        <f>A37</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G37" s="8">
@@ -28580,7 +28543,7 @@
         <v>8.3333333333333037E-3</v>
       </c>
       <c r="D38" s="8" t="str">
-        <f>A38</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E38" s="8">
@@ -28588,7 +28551,7 @@
         <v>2.2916666666666696E-2</v>
       </c>
       <c r="F38" s="8" t="str">
-        <f>A38</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G38" s="8">
@@ -28610,7 +28573,7 @@
         <v>5.5555555555555358E-3</v>
       </c>
       <c r="D39" s="8" t="str">
-        <f>A39</f>
+        <f t="shared" si="0"/>
         <v>Student</v>
       </c>
       <c r="E39" s="8">
@@ -28618,7 +28581,7 @@
         <v>2.430555555555558E-2</v>
       </c>
       <c r="F39" s="8" t="str">
-        <f>A39</f>
+        <f t="shared" si="1"/>
         <v>Student</v>
       </c>
       <c r="G39" s="8">
@@ -28640,7 +28603,7 @@
         <v>3.4722222222222099E-3</v>
       </c>
       <c r="D40" s="8" t="str">
-        <f>A40</f>
+        <f t="shared" si="0"/>
         <v>Industry Professional</v>
       </c>
       <c r="E40" s="8">
@@ -28648,7 +28611,7 @@
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="F40" s="8" t="str">
-        <f>A40</f>
+        <f t="shared" si="1"/>
         <v>Industry Professional</v>
       </c>
       <c r="G40" s="8">
@@ -28670,7 +28633,7 @@
         <v>1.1111111111111072E-2</v>
       </c>
       <c r="D41" s="8" t="str">
-        <f>A41</f>
+        <f t="shared" si="0"/>
         <v>Industry Professional</v>
       </c>
       <c r="E41" s="8">
@@ -28678,7 +28641,7 @@
         <v>9.0277777777777457E-3</v>
       </c>
       <c r="F41" s="8" t="str">
-        <f>A41</f>
+        <f t="shared" si="1"/>
         <v>Industry Professional</v>
       </c>
       <c r="G41" s="8">
@@ -28700,7 +28663,7 @@
         <v>5.5555555555555358E-3</v>
       </c>
       <c r="D42" s="8" t="str">
-        <f>A42</f>
+        <f t="shared" si="0"/>
         <v>Industry Professional</v>
       </c>
       <c r="E42" s="8">
@@ -28708,7 +28671,7 @@
         <v>1.1111111111111072E-2</v>
       </c>
       <c r="F42" s="8" t="str">
-        <f>A42</f>
+        <f t="shared" si="1"/>
         <v>Industry Professional</v>
       </c>
       <c r="G42" s="8">
@@ -28730,7 +28693,7 @@
         <v>7.6388888888889173E-3</v>
       </c>
       <c r="D43" s="8" t="str">
-        <f>A43</f>
+        <f t="shared" si="0"/>
         <v>Industry Professional</v>
       </c>
       <c r="E43" s="8">
@@ -28738,7 +28701,7 @@
         <v>1.8749999999999933E-2</v>
       </c>
       <c r="F43" s="8" t="str">
-        <f>A43</f>
+        <f t="shared" si="1"/>
         <v>Industry Professional</v>
       </c>
       <c r="G43" s="8">
@@ -28760,7 +28723,7 @@
         <v>6.9444444444444198E-4</v>
       </c>
       <c r="D44" s="8" t="str">
-        <f>A44</f>
+        <f t="shared" si="0"/>
         <v>Researcher</v>
       </c>
       <c r="E44" s="8">
@@ -28768,7 +28731,7 @@
         <v>2.2916666666666585E-2</v>
       </c>
       <c r="F44" s="8" t="str">
-        <f>A44</f>
+        <f t="shared" si="1"/>
         <v>Researcher</v>
       </c>
       <c r="G44" s="8">
@@ -28790,8 +28753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{168FCA7C-DF0F-4DB4-A6C7-395CDDD91BBA}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q37" sqref="Q37"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
adapted chart formatting for ranking
</commit_message>
<xml_diff>
--- a/UserTestEval/Data/Rawdata.xlsx
+++ b/UserTestEval/Data/Rawdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katha\Documents\uni\Evaluation-of-templates-for-requirements-documentation\UserTestEval\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C708F31F-0FBE-4248-81C0-08793358F8C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5842710-C390-4081-A7A0-1695BE0BD509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40920" yWindow="3975" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,80 +21,63 @@
     <sheet name="QualityReview" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Ranking!$A$2:$A$211</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Ranking!$A$2:$A$216</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Ranking!$B$1</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Ranking!$C$2:$C$216</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Ranking!$D$1</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Ranking!$D$2:$D$216</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Ranking!$A$2:$A$216</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Ranking!$C$1</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Ranking!$C$2:$C$211</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Ranking!$D$1</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Ranking!$D$2:$D$211</definedName>
     <definedName name="_xlchart.v1.14" hidden="1">Ranking!$B$1</definedName>
     <definedName name="_xlchart.v1.15" hidden="1">Ranking!$B$2:$B$216</definedName>
     <definedName name="_xlchart.v1.16" hidden="1">Ranking!$C$1</definedName>
     <definedName name="_xlchart.v1.17" hidden="1">Ranking!$C$2:$C$216</definedName>
     <definedName name="_xlchart.v1.18" hidden="1">Ranking!$D$1</definedName>
     <definedName name="_xlchart.v1.19" hidden="1">Ranking!$D$2:$D$216</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Ranking!$B$2:$B$211</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Ranking!$B$1</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Ranking!$B$2:$B$216</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Ranking!$C$1</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Ranking!$C$2:$C$216</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Ranking!$D$1</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Ranking!$D$2:$D$216</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Ranking!$A$2:$A$211</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">Ranking!$B$1</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">Ranking!$B$2:$B$211</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">Ranking!$C$1</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Ranking!$B$2:$B$216</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">Time!$A$2:$A$43</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Time!$B$1</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">Time!$B$2:$B$43</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">Time!$C$1</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">Time!$C$2:$C$43</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">Time!$F$2:$F$43</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">Time!$G$1</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">Time!$G$2:$G$43</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">Time!$A$2:$A$44</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">Time!$B$1</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">Ranking!$C$1</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">Ranking!$C$2:$C$211</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">Ranking!$D$1</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">Ranking!$D$2:$D$211</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">Time!$B$2:$B$44</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">Time!$C$1</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">Time!$C$2:$C$44</definedName>
     <definedName name="_xlchart.v1.33" hidden="1">Time!$D$3:$D$43</definedName>
     <definedName name="_xlchart.v1.34" hidden="1">Time!$E$3:$E$43</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">Time!$D$3:$D$43</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">Time!$E$3:$E$43</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">Time!$A$2:$A$43</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">Time!$B$1</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">Time!$B$2:$B$43</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Ranking!$C$2:$C$211</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">Time!$C$1</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">Time!$C$2:$C$43</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">Time!$F$2:$F$43</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">Time!$G$1</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">Time!$G$2:$G$43</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">Time!$D$3:$D$43</definedName>
-    <definedName name="_xlchart.v1.46" hidden="1">Time!$E$3:$E$43</definedName>
-    <definedName name="_xlchart.v1.47" hidden="1">Time!$A$2:$A$44</definedName>
-    <definedName name="_xlchart.v1.48" hidden="1">Time!$B$1</definedName>
-    <definedName name="_xlchart.v1.49" hidden="1">Time!$B$2:$B$44</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">QualityReview!$A$2:$B$13</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">QualityReview!$C$1</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">QualityReview!$C$2:$C$13</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">QualityReview!$D$1</definedName>
+    <definedName name="_xlchart.v1.39" hidden="1">QualityReview!$D$2:$D$13</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Ranking!$C$2:$C$216</definedName>
+    <definedName name="_xlchart.v1.40" hidden="1">QualityReview!$E$1</definedName>
+    <definedName name="_xlchart.v1.41" hidden="1">QualityReview!$E$2:$E$13</definedName>
+    <definedName name="_xlchart.v1.42" hidden="1">QualityReview!$F$1</definedName>
+    <definedName name="_xlchart.v1.43" hidden="1">QualityReview!$F$2:$F$13</definedName>
+    <definedName name="_xlchart.v1.44" hidden="1">QualityReview!$G$1</definedName>
+    <definedName name="_xlchart.v1.45" hidden="1">QualityReview!$G$2:$G$13</definedName>
+    <definedName name="_xlchart.v1.46" hidden="1">QualityReview!$A$23:$A$34</definedName>
+    <definedName name="_xlchart.v1.47" hidden="1">QualityReview!$C$22</definedName>
+    <definedName name="_xlchart.v1.48" hidden="1">QualityReview!$C$23:$C$34</definedName>
+    <definedName name="_xlchart.v1.49" hidden="1">QualityReview!$D$22</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">Ranking!$D$1</definedName>
-    <definedName name="_xlchart.v1.50" hidden="1">Time!$C$1</definedName>
-    <definedName name="_xlchart.v1.51" hidden="1">Time!$C$2:$C$44</definedName>
-    <definedName name="_xlchart.v1.52" hidden="1">QualityReview!$A$2:$B$13</definedName>
-    <definedName name="_xlchart.v1.53" hidden="1">QualityReview!$C$1</definedName>
-    <definedName name="_xlchart.v1.54" hidden="1">QualityReview!$C$2:$C$13</definedName>
-    <definedName name="_xlchart.v1.55" hidden="1">QualityReview!$D$1</definedName>
-    <definedName name="_xlchart.v1.56" hidden="1">QualityReview!$D$2:$D$13</definedName>
-    <definedName name="_xlchart.v1.57" hidden="1">QualityReview!$E$1</definedName>
-    <definedName name="_xlchart.v1.58" hidden="1">QualityReview!$E$2:$E$13</definedName>
-    <definedName name="_xlchart.v1.59" hidden="1">QualityReview!$F$1</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Ranking!$D$2:$D$211</definedName>
-    <definedName name="_xlchart.v1.60" hidden="1">QualityReview!$F$2:$F$13</definedName>
-    <definedName name="_xlchart.v1.61" hidden="1">QualityReview!$G$1</definedName>
-    <definedName name="_xlchart.v1.62" hidden="1">QualityReview!$G$2:$G$13</definedName>
-    <definedName name="_xlchart.v1.63" hidden="1">QualityReview!$A$23:$A$34</definedName>
-    <definedName name="_xlchart.v1.64" hidden="1">QualityReview!$C$22</definedName>
-    <definedName name="_xlchart.v1.65" hidden="1">QualityReview!$C$23:$C$34</definedName>
-    <definedName name="_xlchart.v1.66" hidden="1">QualityReview!$D$22</definedName>
-    <definedName name="_xlchart.v1.67" hidden="1">QualityReview!$D$23:$D$34</definedName>
-    <definedName name="_xlchart.v1.68" hidden="1">QualityReview!$E$22</definedName>
-    <definedName name="_xlchart.v1.69" hidden="1">QualityReview!$E$23:$E$34</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Ranking!$B$1</definedName>
-    <definedName name="_xlchart.v1.70" hidden="1">QualityReview!$F$22</definedName>
-    <definedName name="_xlchart.v1.71" hidden="1">QualityReview!$F$23:$F$34</definedName>
-    <definedName name="_xlchart.v1.72" hidden="1">QualityReview!$G$22</definedName>
-    <definedName name="_xlchart.v1.73" hidden="1">QualityReview!$G$23:$G$34</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Ranking!$B$2:$B$216</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Ranking!$C$1</definedName>
+    <definedName name="_xlchart.v1.50" hidden="1">QualityReview!$D$23:$D$34</definedName>
+    <definedName name="_xlchart.v1.51" hidden="1">QualityReview!$E$22</definedName>
+    <definedName name="_xlchart.v1.52" hidden="1">QualityReview!$E$23:$E$34</definedName>
+    <definedName name="_xlchart.v1.53" hidden="1">QualityReview!$F$22</definedName>
+    <definedName name="_xlchart.v1.54" hidden="1">QualityReview!$F$23:$F$34</definedName>
+    <definedName name="_xlchart.v1.55" hidden="1">QualityReview!$G$22</definedName>
+    <definedName name="_xlchart.v1.56" hidden="1">QualityReview!$G$23:$G$34</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Ranking!$D$2:$D$216</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Ranking!$A$2:$A$211</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Ranking!$B$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Ranking!$B$2:$B$211</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -5661,17 +5644,17 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.21</cx:f>
+        <cx:f>_xlchart.v1.15</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.23</cx:f>
+        <cx:f>_xlchart.v1.17</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.25</cx:f>
+        <cx:f>_xlchart.v1.19</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5681,7 +5664,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{DFFD1D8C-500C-4E2A-9211-797C479ECBE1}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.20</cx:f>
+              <cx:f>_xlchart.v1.14</cx:f>
               <cx:v>free</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5694,7 +5677,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{98B69223-0ACB-44C9-9018-FA832260212A}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.22</cx:f>
+              <cx:f>_xlchart.v1.16</cx:f>
               <cx:v>EARS</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5707,7 +5690,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{F4DD60D6-E854-4988-8C74-F33CFDB1A5CD}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.24</cx:f>
+              <cx:f>_xlchart.v1.18</cx:f>
               <cx:v>MASTER</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5757,7 +5740,7 @@
         <cx:title>
           <cx:tx>
             <cx:txData>
-              <cx:v>worst ⟝ --                         -- ⟞ best</cx:v>
+              <cx:v>worst ⟝ --       -- ⟞ best</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:txPr>
@@ -5765,7 +5748,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-                <a:defRPr lang="en-DE" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:defRPr lang="en-DE" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:sysClr val="windowText" lastClr="000000">
                       <a:lumMod val="65000"/>
@@ -5778,7 +5761,7 @@
                 </a:defRPr>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-DE" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-DE" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:sysClr val="windowText" lastClr="000000">
                       <a:lumMod val="65000"/>
@@ -5789,7 +5772,7 @@
                   <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                   <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                 </a:rPr>
-                <a:t>worst ⟝ --                         -- ⟞ best</a:t>
+                <a:t>worst ⟝ --       -- ⟞ best</a:t>
               </a:r>
             </a:p>
           </cx:txPr>
@@ -5801,7 +5784,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr" rtl="0">
-              <a:defRPr lang="en-DE" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:defRPr lang="en-DE" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000">
                     <a:lumMod val="65000"/>
@@ -5813,7 +5796,7 @@
                 <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-DE" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0">
+            <a:endParaRPr lang="en-DE" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000">
                   <a:lumMod val="65000"/>
@@ -5869,7 +5852,7 @@
   <cx:printSettings>
     <cx:headerFooter alignWithMargins="1" differentOddEven="0" differentFirst="0"/>
     <cx:pageMargins l="0" r="0" t="0" b="0" header="0" footer="0"/>
-    <cx:pageSetup paperSize="1" firstPageNumber="1" orientation="landscape" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
+    <cx:pageSetup paperSize="1" firstPageNumber="1" orientation="portrait" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
   </cx:printSettings>
 </cx:chartSpace>
 </file>
@@ -5879,26 +5862,26 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.13</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.15</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.13</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.17</cx:f>
+        <cx:f>_xlchart.v1.4</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.13</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.19</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5915,7 +5898,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{9F5367F5-9D47-46AD-B596-0EFA7A478491}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.14</cx:f>
+              <cx:f>_xlchart.v1.1</cx:f>
               <cx:v>free</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5928,7 +5911,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{5A5F7C4B-719B-40B2-B332-D53E44E122AB}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.16</cx:f>
+              <cx:f>_xlchart.v1.3</cx:f>
               <cx:v>EARS</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5941,7 +5924,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{55F26920-8301-4343-A252-521020BA38E7}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.18</cx:f>
+              <cx:f>_xlchart.v1.5</cx:f>
               <cx:v>MASTER</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6159,26 +6142,26 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.26</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.28</cx:f>
+        <cx:f>_xlchart.v1.9</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.26</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.30</cx:f>
+        <cx:f>_xlchart.v1.11</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.26</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.32</cx:f>
+        <cx:f>_xlchart.v1.13</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -6195,7 +6178,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{CB637DB2-7F16-46BD-BECF-B186D777151E}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.27</cx:f>
+              <cx:f>_xlchart.v1.8</cx:f>
               <cx:v>free</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6208,7 +6191,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{C908A5A9-6C1E-4C60-B384-5224CE0FDF11}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.29</cx:f>
+              <cx:f>_xlchart.v1.10</cx:f>
               <cx:v>EARS</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6221,7 +6204,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{B19EAA18-68A6-4A27-8698-E85CD5441D2F}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.31</cx:f>
+              <cx:f>_xlchart.v1.12</cx:f>
               <cx:v>MASTER</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6240,7 +6223,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr" rtl="0">
-              <a:defRPr lang="en-DE" sz="1100" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:defRPr lang="en-DE" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000">
                     <a:lumMod val="65000"/>
@@ -6252,7 +6235,7 @@
                 <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-DE" sz="1100" b="1" i="0" u="none" strike="noStrike" baseline="0">
+            <a:endParaRPr lang="en-DE" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000">
                   <a:lumMod val="65000"/>
@@ -6270,81 +6253,30 @@
         <cx:valScaling/>
         <cx:title>
           <cx:tx>
-            <cx:rich>
-              <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-                  <a:lnSpc>
-                    <a:spcPct val="100000"/>
-                  </a:lnSpc>
-                  <a:spcBef>
-                    <a:spcPts val="0"/>
-                  </a:spcBef>
-                  <a:spcAft>
-                    <a:spcPts val="0"/>
-                  </a:spcAft>
-                  <a:buClrTx/>
-                  <a:buSzTx/>
-                  <a:buFontTx/>
-                  <a:buNone/>
-                  <a:tabLst/>
-                  <a:defRPr lang="en-DE" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:sysClr>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-                    <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-DE" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:sysClr>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-                    <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                  </a:rPr>
-                  <a:t>worst ⟝ --                         -- ⟞ best</a:t>
-                </a:r>
-              </a:p>
-              <a:p>
-                <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-                  <a:lnSpc>
-                    <a:spcPct val="100000"/>
-                  </a:lnSpc>
-                  <a:spcBef>
-                    <a:spcPts val="0"/>
-                  </a:spcBef>
-                  <a:spcAft>
-                    <a:spcPts val="0"/>
-                  </a:spcAft>
-                  <a:buClrTx/>
-                  <a:buSzTx/>
-                  <a:buFontTx/>
-                  <a:buNone/>
-                  <a:tabLst/>
-                  <a:defRPr lang="en-DE" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:sysClr>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-                    <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-DE" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0">
+            <cx:txData>
+              <cx:v>worst ⟝ --          -- ⟞ best</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr lang="en-DE" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:sysClr val="windowText" lastClr="000000">
                       <a:lumMod val="65000"/>
@@ -6354,10 +6286,24 @@
                   <a:latin typeface="Calibri" panose="020F0502020204030204"/>
                   <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
                   <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                </a:endParaRPr>
-              </a:p>
-            </cx:rich>
-          </cx:tx>
+                </a:defRPr>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-DE" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                  <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>worst ⟝ --          -- ⟞ best</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
         </cx:title>
         <cx:majorGridlines/>
         <cx:tickLabels/>
@@ -6366,7 +6312,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr" rtl="0">
-              <a:defRPr lang="en-DE" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:defRPr lang="en-DE" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000">
                     <a:lumMod val="65000"/>
@@ -6378,7 +6324,7 @@
                 <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-DE" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:endParaRPr lang="en-DE" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000">
                   <a:lumMod val="65000"/>
@@ -6434,7 +6380,7 @@
   <cx:printSettings>
     <cx:headerFooter alignWithMargins="1" differentOddEven="0" differentFirst="0"/>
     <cx:pageMargins l="0" r="0" t="0" b="0" header="0" footer="0"/>
-    <cx:pageSetup paperSize="1" firstPageNumber="1" orientation="landscape" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
+    <cx:pageSetup paperSize="1" firstPageNumber="1" orientation="portrait" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
   </cx:printSettings>
 </cx:chartSpace>
 </file>
@@ -6444,18 +6390,18 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.47</cx:f>
+        <cx:f>_xlchart.v1.28</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.49</cx:f>
+        <cx:f>_xlchart.v1.30</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.47</cx:f>
+        <cx:f>_xlchart.v1.28</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.51</cx:f>
+        <cx:f>_xlchart.v1.32</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -6465,7 +6411,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{A7955AD6-7364-416F-A82A-58A1F76E455D}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.48</cx:f>
+              <cx:f>_xlchart.v1.29</cx:f>
               <cx:v>EARS</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6490,7 +6436,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{6C77626C-2690-4B4A-A861-13008AE16954}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.50</cx:f>
+              <cx:f>_xlchart.v1.31</cx:f>
               <cx:v>MASTER</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6538,18 +6484,18 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.37</cx:f>
+        <cx:f>_xlchart.v1.20</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.39</cx:f>
+        <cx:f>_xlchart.v1.22</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.37</cx:f>
+        <cx:f>_xlchart.v1.20</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.41</cx:f>
+        <cx:f>_xlchart.v1.24</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -6559,7 +6505,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{F8EE3ECA-F2A0-4D89-B44B-860DB1DF4BFB}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.38</cx:f>
+              <cx:f>_xlchart.v1.21</cx:f>
               <cx:v>EARS</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6584,7 +6530,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{5FE71DA6-CBA9-45DB-9983-296628AFA7E5}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.40</cx:f>
+              <cx:f>_xlchart.v1.23</cx:f>
               <cx:v>MASTER</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6696,10 +6642,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.42</cx:f>
+        <cx:f>_xlchart.v1.25</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.44</cx:f>
+        <cx:f>_xlchart.v1.27</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -6716,7 +6662,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{4F766D4F-6C7B-48A5-BD5A-CAC0903FDF09}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.43</cx:f>
+              <cx:f>_xlchart.v1.26</cx:f>
               <cx:v>Total</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6752,10 +6698,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.45</cx:f>
+        <cx:f>_xlchart.v1.33</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.46</cx:f>
+        <cx:f>_xlchart.v1.34</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -6895,7 +6841,7 @@
   <cx:printSettings>
     <cx:headerFooter alignWithMargins="1" differentOddEven="0" differentFirst="0"/>
     <cx:pageMargins l="0" r="0" t="0" b="0" header="0" footer="0"/>
-    <cx:pageSetup paperSize="3" firstPageNumber="1" orientation="landscape" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
+    <cx:pageSetup paperSize="1" firstPageNumber="1" orientation="default" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
   </cx:printSettings>
 </cx:chartSpace>
 </file>
@@ -6905,42 +6851,42 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.52</cx:f>
+        <cx:f>_xlchart.v1.35</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.54</cx:f>
+        <cx:f>_xlchart.v1.37</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.52</cx:f>
+        <cx:f>_xlchart.v1.35</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.56</cx:f>
+        <cx:f>_xlchart.v1.39</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.52</cx:f>
+        <cx:f>_xlchart.v1.35</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.58</cx:f>
+        <cx:f>_xlchart.v1.41</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.52</cx:f>
+        <cx:f>_xlchart.v1.35</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.60</cx:f>
+        <cx:f>_xlchart.v1.43</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="4">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.52</cx:f>
+        <cx:f>_xlchart.v1.35</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.62</cx:f>
+        <cx:f>_xlchart.v1.45</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -6950,7 +6896,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{4C9521D1-631F-42F0-9749-FB8937F087F6}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.53</cx:f>
+              <cx:f>_xlchart.v1.36</cx:f>
               <cx:v>vague</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6963,7 +6909,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{9AF2D6D6-5CAF-49D2-9B24-3FDC5856B60B}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.55</cx:f>
+              <cx:f>_xlchart.v1.38</cx:f>
               <cx:v>incomplete</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6976,7 +6922,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{73B81BD9-37F7-49AC-B2E8-F54E906408DE}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.57</cx:f>
+              <cx:f>_xlchart.v1.40</cx:f>
               <cx:v>incorrect</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6989,7 +6935,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{B5BD30F9-3ACC-4B38-AE2B-3C3A90D468E8}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.59</cx:f>
+              <cx:f>_xlchart.v1.42</cx:f>
               <cx:v>inconcise</cx:v>
             </cx:txData>
           </cx:tx>
@@ -7002,7 +6948,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{6A7141D9-821B-43D6-A511-20B9A837316A}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.61</cx:f>
+              <cx:f>_xlchart.v1.44</cx:f>
               <cx:v>none</cx:v>
             </cx:txData>
           </cx:tx>
@@ -7197,42 +7143,42 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.63</cx:f>
+        <cx:f>_xlchart.v1.46</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.65</cx:f>
+        <cx:f>_xlchart.v1.48</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.63</cx:f>
+        <cx:f>_xlchart.v1.46</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.67</cx:f>
+        <cx:f>_xlchart.v1.50</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.63</cx:f>
+        <cx:f>_xlchart.v1.46</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.69</cx:f>
+        <cx:f>_xlchart.v1.52</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.63</cx:f>
+        <cx:f>_xlchart.v1.46</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.71</cx:f>
+        <cx:f>_xlchart.v1.54</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="4">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.63</cx:f>
+        <cx:f>_xlchart.v1.46</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.73</cx:f>
+        <cx:f>_xlchart.v1.56</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -7242,7 +7188,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{8B770BCC-FD5C-4D68-AEEB-508E9CF72DCE}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.64</cx:f>
+              <cx:f>_xlchart.v1.47</cx:f>
               <cx:v>vague</cx:v>
             </cx:txData>
           </cx:tx>
@@ -7255,7 +7201,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{291446AC-771A-4D6C-A698-7EF520B42796}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.66</cx:f>
+              <cx:f>_xlchart.v1.49</cx:f>
               <cx:v>incomplete</cx:v>
             </cx:txData>
           </cx:tx>
@@ -7268,7 +7214,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{51452AC8-4C76-4012-8B1F-68B36AD3A0E8}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.68</cx:f>
+              <cx:f>_xlchart.v1.51</cx:f>
               <cx:v>incorrect</cx:v>
             </cx:txData>
           </cx:tx>
@@ -7281,7 +7227,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{B0886783-8255-4C29-A357-F9361D617F60}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.70</cx:f>
+              <cx:f>_xlchart.v1.53</cx:f>
               <cx:v>inconcise</cx:v>
             </cx:txData>
           </cx:tx>
@@ -7294,7 +7240,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{7F7349DE-A086-4B3F-9A26-501C2B73C7A8}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.72</cx:f>
+              <cx:f>_xlchart.v1.55</cx:f>
               <cx:v>none</cx:v>
             </cx:txData>
           </cx:tx>
@@ -16833,13 +16779,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
+      <xdr:colOff>523876</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>485774</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>114301</xdr:rowOff>
     </xdr:to>
@@ -16877,8 +16823,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3876675" y="3267075"/>
-              <a:ext cx="3314699" cy="2686051"/>
+              <a:off x="3876676" y="3267075"/>
+              <a:ext cx="2524124" cy="2686051"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -16989,13 +16935,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
+      <xdr:colOff>514351</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
@@ -17033,8 +16979,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3867150" y="6105525"/>
-              <a:ext cx="3295650" cy="2838450"/>
+              <a:off x="3867151" y="6105525"/>
+              <a:ext cx="2533649" cy="2838450"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -29216,7 +29162,7 @@
   <dimension ref="A1:D216"/>
   <sheetViews>
     <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
added t-tests for significance analysis
</commit_message>
<xml_diff>
--- a/UserTestEval/Data/Rawdata.xlsx
+++ b/UserTestEval/Data/Rawdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katha\Documents\uni\Evaluation-of-templates-for-requirements-documentation\UserTestEval\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5842710-C390-4081-A7A0-1695BE0BD509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BDF0589-BBE2-4935-A6E1-EE3C511154BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="3975" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40920" yWindow="3975" windowWidth="25440" windowHeight="15270" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AllData" sheetId="2" r:id="rId1"/>
@@ -21,19 +21,19 @@
     <sheet name="QualityReview" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Ranking!$A$2:$A$216</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Ranking!$A$2:$A$211</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Ranking!$B$1</definedName>
     <definedName name="_xlchart.v1.10" hidden="1">Ranking!$C$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Ranking!$C$2:$C$211</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Ranking!$C$2:$C$216</definedName>
     <definedName name="_xlchart.v1.12" hidden="1">Ranking!$D$1</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Ranking!$D$2:$D$211</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Ranking!$D$2:$D$216</definedName>
     <definedName name="_xlchart.v1.14" hidden="1">Ranking!$B$1</definedName>
     <definedName name="_xlchart.v1.15" hidden="1">Ranking!$B$2:$B$216</definedName>
     <definedName name="_xlchart.v1.16" hidden="1">Ranking!$C$1</definedName>
     <definedName name="_xlchart.v1.17" hidden="1">Ranking!$C$2:$C$216</definedName>
     <definedName name="_xlchart.v1.18" hidden="1">Ranking!$D$1</definedName>
     <definedName name="_xlchart.v1.19" hidden="1">Ranking!$D$2:$D$216</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Ranking!$B$2:$B$216</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Ranking!$B$2:$B$211</definedName>
     <definedName name="_xlchart.v1.20" hidden="1">Time!$A$2:$A$43</definedName>
     <definedName name="_xlchart.v1.21" hidden="1">Time!$B$1</definedName>
     <definedName name="_xlchart.v1.22" hidden="1">Time!$B$2:$B$43</definedName>
@@ -55,7 +55,7 @@
     <definedName name="_xlchart.v1.37" hidden="1">QualityReview!$C$2:$C$13</definedName>
     <definedName name="_xlchart.v1.38" hidden="1">QualityReview!$D$1</definedName>
     <definedName name="_xlchart.v1.39" hidden="1">QualityReview!$D$2:$D$13</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Ranking!$C$2:$C$216</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Ranking!$C$2:$C$211</definedName>
     <definedName name="_xlchart.v1.40" hidden="1">QualityReview!$E$1</definedName>
     <definedName name="_xlchart.v1.41" hidden="1">QualityReview!$E$2:$E$13</definedName>
     <definedName name="_xlchart.v1.42" hidden="1">QualityReview!$F$1</definedName>
@@ -74,10 +74,10 @@
     <definedName name="_xlchart.v1.54" hidden="1">QualityReview!$F$23:$F$34</definedName>
     <definedName name="_xlchart.v1.55" hidden="1">QualityReview!$G$22</definedName>
     <definedName name="_xlchart.v1.56" hidden="1">QualityReview!$G$23:$G$34</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Ranking!$D$2:$D$216</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Ranking!$A$2:$A$211</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Ranking!$D$2:$D$211</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Ranking!$A$2:$A$216</definedName>
     <definedName name="_xlchart.v1.8" hidden="1">Ranking!$B$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Ranking!$B$2:$B$211</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Ranking!$B$2:$B$216</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -98,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2019" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2059" uniqueCount="279">
   <si>
     <t>What is your occupation?</t>
   </si>
@@ -898,12 +898,54 @@
   <si>
     <t>Professional</t>
   </si>
+  <si>
+    <t>σ EARS</t>
+  </si>
+  <si>
+    <t>σ MASTER</t>
+  </si>
+  <si>
+    <t>σ free</t>
+  </si>
+  <si>
+    <t>t-test EARS</t>
+  </si>
+  <si>
+    <t>t-test MASTER</t>
+  </si>
+  <si>
+    <t>t-test EARS vs MASTER</t>
+  </si>
+  <si>
+    <t>Students</t>
+  </si>
+  <si>
+    <t>Professionals</t>
+  </si>
+  <si>
+    <t>vs Students</t>
+  </si>
+  <si>
+    <t>Writingtime</t>
+  </si>
+  <si>
+    <t>Reviewtime</t>
+  </si>
+  <si>
+    <t>σ Students</t>
+  </si>
+  <si>
+    <t>σ Professionals</t>
+  </si>
+  <si>
+    <t>t-test</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -922,6 +964,14 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -959,7 +1009,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -979,6 +1029,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -5852,7 +5904,7 @@
   <cx:printSettings>
     <cx:headerFooter alignWithMargins="1" differentOddEven="0" differentFirst="0"/>
     <cx:pageMargins l="0" r="0" t="0" b="0" header="0" footer="0"/>
-    <cx:pageSetup paperSize="1" firstPageNumber="1" orientation="portrait" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
+    <cx:pageSetup paperSize="1" firstPageNumber="1" orientation="default" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
   </cx:printSettings>
 </cx:chartSpace>
 </file>
@@ -5862,26 +5914,26 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.9</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.4</cx:f>
+        <cx:f>_xlchart.v1.11</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.13</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5898,7 +5950,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{9F5367F5-9D47-46AD-B596-0EFA7A478491}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.1</cx:f>
+              <cx:f>_xlchart.v1.8</cx:f>
               <cx:v>free</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5911,7 +5963,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{5A5F7C4B-719B-40B2-B332-D53E44E122AB}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.3</cx:f>
+              <cx:f>_xlchart.v1.10</cx:f>
               <cx:v>EARS</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5924,7 +5976,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{55F26920-8301-4343-A252-521020BA38E7}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.5</cx:f>
+              <cx:f>_xlchart.v1.12</cx:f>
               <cx:v>MASTER</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6142,26 +6194,26 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.11</cx:f>
+        <cx:f>_xlchart.v1.4</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.13</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -6178,7 +6230,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{CB637DB2-7F16-46BD-BECF-B186D777151E}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.8</cx:f>
+              <cx:f>_xlchart.v1.1</cx:f>
               <cx:v>free</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6191,7 +6243,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{C908A5A9-6C1E-4C60-B384-5224CE0FDF11}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.10</cx:f>
+              <cx:f>_xlchart.v1.3</cx:f>
               <cx:v>EARS</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6204,7 +6256,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{B19EAA18-68A6-4A27-8698-E85CD5441D2F}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.12</cx:f>
+              <cx:f>_xlchart.v1.5</cx:f>
               <cx:v>MASTER</cx:v>
             </cx:txData>
           </cx:tx>
@@ -6380,7 +6432,7 @@
   <cx:printSettings>
     <cx:headerFooter alignWithMargins="1" differentOddEven="0" differentFirst="0"/>
     <cx:pageMargins l="0" r="0" t="0" b="0" header="0" footer="0"/>
-    <cx:pageSetup paperSize="1" firstPageNumber="1" orientation="portrait" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
+    <cx:pageSetup paperSize="1" firstPageNumber="1" orientation="default" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
   </cx:printSettings>
 </cx:chartSpace>
 </file>
@@ -17017,16 +17069,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>809625</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -17062,8 +17114,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6677025" y="457200"/>
-              <a:ext cx="4572000" cy="2743200"/>
+              <a:off x="10163175" y="3943350"/>
+              <a:ext cx="4572000" cy="2809875"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -18694,7 +18746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BS44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -29159,15 +29211,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11A71970-3F06-4A38-BA8F-62028407EBDC}">
-  <dimension ref="A1:D216"/>
+  <dimension ref="A1:M216"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="11" max="11" width="17.875" customWidth="1"/>
+    <col min="12" max="12" width="11.5" customWidth="1"/>
+    <col min="13" max="13" width="14.25" customWidth="1"/>
+    <col min="14" max="14" width="12.125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A1" s="6" t="s">
         <v>256</v>
       </c>
@@ -29180,8 +29238,17 @@
       <c r="D1" s="6" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="K1" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="str">
         <f>AllData!A2</f>
         <v>Student</v>
@@ -29198,8 +29265,20 @@
         <f>AllData!K2</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="K2">
+        <f>_xlfn.STDEV.P(B2:B216)</f>
+        <v>1.3741332879787982</v>
+      </c>
+      <c r="L2">
+        <f>_xlfn.STDEV.P(C2:C216)</f>
+        <v>1.1180799426909069</v>
+      </c>
+      <c r="M2">
+        <f>_xlfn.STDEV.P(D2:D216)</f>
+        <v>1.2256144914113893</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" t="str">
         <f>AllData!A5</f>
         <v>Student</v>
@@ -29216,8 +29295,17 @@
         <f>AllData!K5</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="K3" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="str">
         <f>AllData!A6</f>
         <v>Student</v>
@@ -29234,8 +29322,20 @@
         <f>AllData!K6</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="K4">
+        <f>IFERROR(_xlfn.T.TEST(D2:D216,C2:C216,2,IF(IF(L2^2&gt;M2^2,(L2^2)/(M2^2),(M2^2)/(L2^2))&lt;IF(L2^2&gt;M2^2,_xlfn.F.INV(0.95,COUNT(D2:D216)-1,COUNT(D2:D216)-1),_xlfn.F.INV(0.95,COUNT(D2:D216)-1,COUNT(D2:D216)-1)),2,3)),1)</f>
+        <v>0.11044241386425566</v>
+      </c>
+      <c r="L4">
+        <f>IFERROR(_xlfn.T.TEST(C2:C216,B2:B216,2,IF(IF(K2^2&gt;L2^2,(K2^2)/(L2^2),(L2^2)/(K2^2))&lt;IF(K2^2&gt;L2^2,_xlfn.F.INV(0.95,COUNT(C2:C216)-1,COUNT(C2:C216)-1),_xlfn.F.INV(0.95,COUNT(C2:C216)-1,COUNT(C2:C216)-1)),2,3)),1)</f>
+        <v>2.9141318949744068E-2</v>
+      </c>
+      <c r="M4">
+        <f>IFERROR(_xlfn.T.TEST(D2:D216,B2:B216,2,IF(IF(K2^2&gt;M2^2,(K2^2)/(M2^2),(M2^2)/(K2^2))&lt;IF(K2^2&gt;M2^2,_xlfn.F.INV(0.95,COUNT(D2:D216)-1,COUNT(D2:D216)-1),_xlfn.F.INV(0.95,COUNT(D2:D216)-1,COUNT(D2:D216)-1)),2,3)),1)</f>
+        <v>4.3256895505295652E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="str">
         <f>AllData!A7</f>
         <v>Student</v>
@@ -29253,7 +29353,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="str">
         <f>AllData!A8</f>
         <v>Student</v>
@@ -29271,7 +29371,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A7" t="str">
         <f>AllData!A9</f>
         <v>Student</v>
@@ -29288,8 +29388,11 @@
         <f>AllData!K9</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="K7" s="9" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A8" t="str">
         <f>AllData!A10</f>
         <v>Student</v>
@@ -29306,8 +29409,17 @@
         <f>AllData!K10</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="K8" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="M8" s="9" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="str">
         <f>AllData!A11</f>
         <v>Student</v>
@@ -29324,8 +29436,20 @@
         <f>AllData!K11</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="K9">
+        <f>_xlfn.STDEV.P(B2:B191)</f>
+        <v>1.38752854279244</v>
+      </c>
+      <c r="L9">
+        <f t="shared" ref="L9:M9" si="0">_xlfn.STDEV.P(C2:C191)</f>
+        <v>1.1266600556008128</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>1.1927760399339196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A10" t="str">
         <f>AllData!A12</f>
         <v>Student</v>
@@ -29342,8 +29466,17 @@
         <f>AllData!K12</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="K10" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="M10" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="str">
         <f>AllData!A13</f>
         <v>Student</v>
@@ -29360,8 +29493,20 @@
         <f>AllData!K13</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="K11">
+        <f>IFERROR(_xlfn.T.TEST(D2:D191,C2:C191,2,IF(IF(L9^2&gt;M9^2,(L9^2)/(M9^2),(M9^2)/(L9^2))&lt;IF(L9^2&gt;M9^2,_xlfn.F.INV(0.95,COUNT(D2:D191)-1,COUNT(D2:D191)-1),_xlfn.F.INV(0.95,COUNT(D2:D191)-1,COUNT(D2:D191)-1)),2,3)),1)</f>
+        <v>0.113217102685869</v>
+      </c>
+      <c r="L11">
+        <f>IFERROR(_xlfn.T.TEST(C2:C191,B2:B191,2,IF(IF(K9^2&gt;L9^2,(K9^2)/(L9^2),(L9^2)/(K9^2))&lt;IF(K9^2&gt;L9^2,_xlfn.F.INV(0.95,COUNT(C2:C191)-1,COUNT(C2:C191)-1),_xlfn.F.INV(0.95,COUNT(C2:C191)-1,COUNT(C2:C191)-1)),2,3)),1)</f>
+        <v>0.13503965753898423</v>
+      </c>
+      <c r="M11">
+        <f>IFERROR(_xlfn.T.TEST(D2:D191,B2:B191,2,IF(IF(K9^2&gt;M9^2,(K9^2)/(M9^2),(M9^2)/(K9^2))&lt;IF(K9^2&gt;M9^2,_xlfn.F.INV(0.95,COUNT(D2:D191)-1,COUNT(D2:D191)-1),_xlfn.F.INV(0.95,COUNT(D2:D191)-1,COUNT(D2:D191)-1)),2,3)),1)</f>
+        <v>4.1209776752591971E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="str">
         <f>AllData!A14</f>
         <v>Student</v>
@@ -29379,7 +29524,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="str">
         <f>AllData!A15</f>
         <v>Student</v>
@@ -29397,7 +29542,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A14" t="str">
         <f>AllData!A16</f>
         <v>Student</v>
@@ -29414,8 +29559,11 @@
         <f>AllData!K16</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="K14" s="9" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A15" t="str">
         <f>AllData!A18</f>
         <v>Student</v>
@@ -29432,8 +29580,17 @@
         <f>AllData!K18</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="K15" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="M15" s="9" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" t="str">
         <f>AllData!A19</f>
         <v>Student</v>
@@ -29450,8 +29607,20 @@
         <f>AllData!K19</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="K16">
+        <f>_xlfn.STDEV.P(B192:B211)</f>
+        <v>1.3219304066402287</v>
+      </c>
+      <c r="L16">
+        <f t="shared" ref="L16:M16" si="1">_xlfn.STDEV.P(C192:C211)</f>
+        <v>0.83666002653407556</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="1"/>
+        <v>1.3518505834595773</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A17" t="str">
         <f>AllData!A20</f>
         <v>Student</v>
@@ -29468,8 +29637,17 @@
         <f>AllData!K20</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="K17" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="L17" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="M17" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" t="str">
         <f>AllData!A21</f>
         <v>Student</v>
@@ -29486,8 +29664,20 @@
         <f>AllData!K21</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="K18">
+        <f>IFERROR(_xlfn.T.TEST(D192:D211,C192:C211,2,IF(IF(L16^2&gt;M16^2,(L16^2)/(M16^2),(M16^2)/(L16^2))&lt;IF(L16^2&gt;M16^2,_xlfn.F.INV(0.95,COUNT(D192:D211)-1,COUNT(D192:D211)-1),_xlfn.F.INV(0.95,COUNT(D192:D211)-1,COUNT(D192:D211)-1)),2,3)),1)</f>
+        <v>0.68364558666092212</v>
+      </c>
+      <c r="L18">
+        <f>IFERROR(_xlfn.T.TEST(C192:C211,B192:B211,2,IF(IF(K16^2&gt;L16^2,(K16^2)/(L16^2),(L16^2)/(K16^2))&lt;IF(K16^2&gt;L16^2,_xlfn.F.INV(0.95,COUNT(C192:C211)-1,COUNT(C192:C211)-1),_xlfn.F.INV(0.95,COUNT(C192:C211)-1,COUNT(C192:C211)-1)),2,3)),1)</f>
+        <v>6.2643195007046678E-3</v>
+      </c>
+      <c r="M18">
+        <f>IFERROR(_xlfn.T.TEST(D192:D211,B192:B211,2,IF(IF(K16^2&gt;M16^2,(K16^2)/(M16^2),(M16^2)/(K16^2))&lt;IF(K16^2&gt;M16^2,_xlfn.F.INV(0.95,COUNT(D192:D211)-1,COUNT(D192:D211)-1),_xlfn.F.INV(0.95,COUNT(D192:D211)-1,COUNT(D192:D211)-1)),2,3)),1)</f>
+        <v>8.703144873302723E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A19" t="str">
         <f>AllData!A22</f>
         <v>Student</v>
@@ -29504,8 +29694,19 @@
         <f>AllData!K22</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="K19" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="L19">
+        <f>IFERROR(_xlfn.T.TEST(C192:C211,C2:C191,2,IF(IF(L9^2&gt;L16^2,(L9^2)/(L16^2),(L16^2)/(L9^2))&lt;IF(L9^2&gt;L16^2,_xlfn.F.INV(0.95,COUNT(C2:C191)-1,COUNT(C192:C211)-1),_xlfn.F.INV(0.95,COUNT(C192:C211)-1,COUNT(C2:C191)-1)),2,3)),1)</f>
+        <v>1.9982420699044965E-2</v>
+      </c>
+      <c r="M19">
+        <f>IFERROR(_xlfn.T.TEST(D192:D211,D2:D191,2,IF(IF(M9^2&gt;M16^2,(M9^2)/(M16^2),(M16^2)/(M9^2))&lt;IF(M9^2&gt;M16^2,_xlfn.F.INV(0.95,COUNT(D2:D191)-1,COUNT(D192:D211)-1),_xlfn.F.INV(0.95,COUNT(D192:D211)-1,COUNT(D2:D191)-1)),2,3)),1)</f>
+        <v>4.680819526160282E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" t="str">
         <f>AllData!A23</f>
         <v>Student</v>
@@ -29523,7 +29724,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="str">
         <f>AllData!A24</f>
         <v>Student</v>
@@ -29541,7 +29742,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" t="str">
         <f>AllData!A25</f>
         <v>Student</v>
@@ -29559,7 +29760,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" t="str">
         <f>AllData!A27</f>
         <v>Student</v>
@@ -29577,7 +29778,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" t="str">
         <f>AllData!A28</f>
         <v>Student</v>
@@ -29595,7 +29796,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" t="str">
         <f>AllData!A29</f>
         <v>Student</v>
@@ -29613,7 +29814,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" t="str">
         <f>AllData!A30</f>
         <v>Student</v>
@@ -29631,7 +29832,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" t="str">
         <f>AllData!A31</f>
         <v>Student</v>
@@ -29649,7 +29850,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" t="str">
         <f>AllData!A32</f>
         <v>Student</v>
@@ -29667,7 +29868,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="str">
         <f>AllData!A33</f>
         <v>Student</v>
@@ -29685,7 +29886,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" t="str">
         <f>AllData!A34</f>
         <v>Student</v>
@@ -29703,7 +29904,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" t="str">
         <f>AllData!A35</f>
         <v>Student</v>
@@ -29721,7 +29922,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" t="str">
         <f>AllData!A37</f>
         <v>Student</v>
@@ -33063,15 +33264,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FC39F50-491B-4545-9F82-98E8A6306DE7}">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:Q44"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="17" max="17" width="12.75" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13.9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A1" s="6" t="s">
         <v>256</v>
       </c>
@@ -33093,8 +33297,27 @@
       <c r="G1" s="6" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J1" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" t="str">
         <f>AllData!A31</f>
         <v>Student</v>
@@ -33123,8 +33346,27 @@
         <f>AllData!I31</f>
         <v>2.9166666666666674E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="L2" s="7">
+        <f>_xlfn.STDEV.P(B2:B44)</f>
+        <v>1.6619464737968959E-3</v>
+      </c>
+      <c r="M2" s="7">
+        <f>_xlfn.STDEV.P(C2:C44)</f>
+        <v>2.1095218162888265E-3</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="P2" s="8">
+        <f>_xlfn.STDEV.P(E3:E39)</f>
+        <v>4.7523916075758767E-3</v>
+      </c>
+      <c r="Q2" s="8">
+        <f>_xlfn.STDEV.P(E40:E43)</f>
+        <v>4.4601502009253774E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" t="str">
         <f>AllData!A11</f>
         <v>Student</v>
@@ -33153,8 +33395,17 @@
         <f>AllData!I11</f>
         <v>6.9444444444445308E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K3" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="O3">
+        <f>IFERROR(_xlfn.T.TEST(E40:E43,E3:E39,2,IF(IF(P2^2&gt;Q2^2,(P2^2)/(Q2^2),(Q2^2)/(P2^2))&lt;IF(P2^2&gt;Q2^2,_xlfn.F.INV(0.95,COUNT(E40:E43)-1,COUNT(E3:E39)-1),_xlfn.F.INV(0.95,COUNT(E3:E39)-1,COUNT(E40:E43)-1)),2,3)),1)</f>
+        <v>0.7339694733541291</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="str">
         <f>SUBSTITUTE(AllData!A3, "Industry ", "")</f>
         <v>Student</v>
@@ -33183,8 +33434,12 @@
         <f>AllData!I3</f>
         <v>1.388888888888884E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K4">
+        <f>IFERROR(_xlfn.T.TEST(B2:B44,C2:C44,2,IF(IF(L2^2&gt;M2^2,(L2^2)/(M2^2),(M2^2)/(L2^2))&lt;IF(L2^2&gt;M2^2,_xlfn.F.INV(0.95,COUNT(B2:B44)-1,COUNT(C2:C44)-1),_xlfn.F.INV(0.95,COUNT(C2:C44)-1,COUNT(B2:B44)-1)),2,3)),1)</f>
+        <v>1.6139826274929523E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="str">
         <f>AllData!A8</f>
         <v>Student</v>
@@ -33214,7 +33469,7 @@
         <v>2.430555555555558E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="str">
         <f>AllData!A18</f>
         <v>Student</v>
@@ -33244,7 +33499,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A7" t="str">
         <f>AllData!A12</f>
         <v>Student</v>
@@ -33273,8 +33528,11 @@
         <f>AllData!I12</f>
         <v>1.8055555555555602E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K7" s="9" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A8" t="str">
         <f>AllData!A16</f>
         <v>Student</v>
@@ -33303,8 +33561,15 @@
         <f>AllData!I16</f>
         <v>2.430555555555558E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K8" s="9"/>
+      <c r="L8" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="M8" s="9" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="str">
         <f>AllData!A4</f>
         <v>Student</v>
@@ -33333,8 +33598,16 @@
         <f>AllData!I4</f>
         <v>1.4583333333333393E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="L9">
+        <f>_xlfn.STDEV.P(B2:B39)</f>
+        <v>1.7170584278576597E-3</v>
+      </c>
+      <c r="M9">
+        <f>_xlfn.STDEV.P(C2:C39)</f>
+        <v>1.8121616311848139E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A10" t="str">
         <f>AllData!A6</f>
         <v>Student</v>
@@ -33363,8 +33636,13 @@
         <f>AllData!I6</f>
         <v>1.8749999999999989E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K10" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" t="str">
         <f>AllData!A2</f>
         <v>Student</v>
@@ -33393,8 +33671,12 @@
         <f>AllData!I2</f>
         <v>1.3888888888888895E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K11">
+        <f>IFERROR(_xlfn.T.TEST(B2:B39,C2:C39,2,IF(IF(L9^2&gt;M9^2,(L9^2)/(M9^2),(M9^2)/(L9^2))&lt;IF(L9^2&gt;M9^2,_xlfn.F.INV(0.95,COUNT(B2:B39)-1,COUNT(C2:C39)-1),_xlfn.F.INV(0.95,COUNT(C2:C39)-1,COUNT(B2:B39)-1)),2,3)),1)</f>
+        <v>5.9395738845493019E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="str">
         <f>AllData!A32</f>
         <v>Student</v>
@@ -33424,7 +33706,7 @@
         <v>1.3194444444444398E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="str">
         <f>AllData!A5</f>
         <v>Student</v>
@@ -33454,7 +33736,7 @@
         <v>1.8749999999999989E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A14" t="str">
         <f>AllData!A19</f>
         <v>Student</v>
@@ -33483,8 +33765,11 @@
         <f>AllData!I19</f>
         <v>1.8055555555555547E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K14" s="9" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A15" t="str">
         <f>AllData!A21</f>
         <v>Student</v>
@@ -33513,8 +33798,15 @@
         <f>AllData!I21</f>
         <v>2.6388888888888851E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K15" s="9"/>
+      <c r="L15" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="M15" s="9" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" t="str">
         <f>AllData!A9</f>
         <v>Student</v>
@@ -33543,8 +33835,16 @@
         <f>AllData!I9</f>
         <v>2.0138888888888873E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="L16">
+        <f>_xlfn.STDEV.P(B40:B43)</f>
+        <v>3.4722222222219323E-4</v>
+      </c>
+      <c r="M16">
+        <f>_xlfn.STDEV.P(C40:C43)</f>
+        <v>2.8208466682763688E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A17" t="str">
         <f>SUBSTITUTE(AllData!A17, "Industry ", "")</f>
         <v>Student</v>
@@ -33573,8 +33873,17 @@
         <f>AllData!I17</f>
         <v>1.7361111111111105E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K17" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="L17" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="M17" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" t="str">
         <f>AllData!A13</f>
         <v>Student</v>
@@ -33603,8 +33912,12 @@
         <f>AllData!I13</f>
         <v>2.2916666666666696E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K18">
+        <f>IFERROR(_xlfn.T.TEST(B40:B43,C40:C43,2,IF(IF(L16^2&gt;M16^2,(L16^2)/(M16^2),(M16^2)/(L16^2))&lt;IF(L16^2&gt;M16^2,_xlfn.F.INV(0.95,COUNT(B40:B43)-1,COUNT(C40:C43)-1),_xlfn.F.INV(0.95,COUNT(C40:C43)-1,COUNT(B40:B43)-1)),2,3)),1)</f>
+        <v>9.9793358724774545E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A19" t="str">
         <f>AllData!A15</f>
         <v>Student</v>
@@ -33633,8 +33946,19 @@
         <f>AllData!I15</f>
         <v>2.777777777777779E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="K19" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="L19">
+        <f>IFERROR(_xlfn.T.TEST(B40:B43,B2:B39,2,IF(IF(L16^2&gt;L9^2,(L16^2)/(L9^2),(L9^2)/(L16^2))&lt;IF(L16^2&gt;L9^2,_xlfn.F.INV(0.95,COUNT(B40:B43)-1,COUNT(B2:B39)-1),_xlfn.F.INV(0.95,COUNT(B2:B39)-1,COUNT(B40:B43)-1)),2,3)),1)</f>
+        <v>1.7534670463685353E-2</v>
+      </c>
+      <c r="M19">
+        <f>IFERROR(_xlfn.T.TEST(C40:C43,C2:C39,2,IF(IF(M16^2&gt;M9^2,(M16^2)/(M9^2),(M9^2)/(M16^2))&lt;IF(M16^2&gt;L9^2,_xlfn.F.INV(0.95,COUNT(C40:C43)-1,COUNT(C2:C39)-1),_xlfn.F.INV(0.95,COUNT(C2:C39)-1,COUNT(C40:C43)-1)),2,3)),1)</f>
+        <v>4.6385722666743089E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" t="str">
         <f>AllData!A10</f>
         <v>Student</v>
@@ -33664,7 +33988,7 @@
         <v>2.0138888888888928E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="str">
         <f>AllData!A7</f>
         <v>Student</v>
@@ -33694,7 +34018,7 @@
         <v>2.0138888888888928E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" t="str">
         <f>AllData!A30</f>
         <v>Student</v>
@@ -33724,7 +34048,7 @@
         <v>1.8750000000000044E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" t="str">
         <f>AllData!A14</f>
         <v>Student</v>
@@ -33754,7 +34078,7 @@
         <v>2.9861111111111116E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" t="str">
         <f>AllData!A20</f>
         <v>Student</v>
@@ -33784,7 +34108,7 @@
         <v>2.5000000000000078E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" t="str">
         <f>AllData!A27</f>
         <v>Student</v>
@@ -33814,7 +34138,7 @@
         <v>1.8750000000000044E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" t="str">
         <f>AllData!A23</f>
         <v>Student</v>
@@ -33844,7 +34168,7 @@
         <v>2.0138888888888928E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" t="str">
         <f>AllData!A25</f>
         <v>Student</v>
@@ -33874,7 +34198,7 @@
         <v>1.8749999999999989E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" t="str">
         <f>SUBSTITUTE(AllData!A26, "Industry ", "")</f>
         <v>Student</v>
@@ -33904,7 +34228,7 @@
         <v>1.8749999999999989E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="str">
         <f>AllData!A24</f>
         <v>Student</v>
@@ -33934,7 +34258,7 @@
         <v>1.9444444444444431E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" t="str">
         <f>AllData!A29</f>
         <v>Student</v>
@@ -33964,7 +34288,7 @@
         <v>2.0833333333333315E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" t="str">
         <f>AllData!A28</f>
         <v>Student</v>
@@ -33994,7 +34318,7 @@
         <v>2.0833333333333315E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" t="str">
         <f>AllData!A39</f>
         <v>Student</v>

</xml_diff>